<commit_message>
End of Lab 4A
</commit_message>
<xml_diff>
--- a/Lab 4/Data.xlsx
+++ b/Lab 4/Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>W moving mass [lb]</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>Amplifier [mA]</t>
+  </si>
+  <si>
+    <t>P Gain</t>
+  </si>
+  <si>
+    <t>Instability</t>
+  </si>
+  <si>
+    <t>f (Hz)</t>
+  </si>
+  <si>
+    <t>10% OS</t>
+  </si>
+  <si>
+    <t>w (rad/s)</t>
   </si>
 </sst>
 </file>
@@ -1075,11 +1090,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Input</a:t>
+              <a:t>Amplifer </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> V vs Flow rate</a:t>
+              <a:t>vs Flow rate</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1513,6 +1528,824 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.2608001702489896E-2"/>
+                  <c:y val="-0.40386043492752183"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-41.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-36.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-32.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-27.599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-13.799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.4499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.1499999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$16:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B596-45EC-961B-D500AC178223}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="395316552"/>
+        <c:axId val="395316880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="395316552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="395316880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="395316880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="395316552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.24043553961695383"/>
+                  <c:y val="-6.4784805209872925E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$30:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$30:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BC40-4143-B8CC-F7F30B763377}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="332588408"/>
+        <c:axId val="332588736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="332588408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="332588736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="332588736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="332588408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1633,6 +2466,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2666,6 +3579,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3268,6 +5213,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3539,10 +5544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,6 +5989,48 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49">
+        <v>4.3049999999999998E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50">
+        <v>0.27050000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed Simulink models and plots (?)
</commit_message>
<xml_diff>
--- a/Lab 4/Data.xlsx
+++ b/Lab 4/Data.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melab2\Desktop\Mechanical-Control-Systems\Lab 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Documents\GitHub\Mechanical Control Systems\Lab 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D029245B-FCFC-4E29-B4EE-35F2C9EABC1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7455"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>W moving mass [lb]</t>
   </si>
@@ -64,11 +72,23 @@
   <si>
     <t>w (rad/s)</t>
   </si>
+  <si>
+    <t>Ramp Steady-State Error</t>
+  </si>
+  <si>
+    <t>Half of Steady-State Error</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>KP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +182,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -577,7 +596,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1100,7 +1118,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1543,7 +1560,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1952,7 +1968,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5143,7 +5158,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5173,7 +5194,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5203,7 +5230,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5233,7 +5266,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5263,7 +5302,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5543,16 +5588,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5563,7 +5608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>22.91</v>
       </c>
@@ -5574,7 +5619,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5582,7 +5627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>-4</v>
       </c>
@@ -5590,7 +5635,7 @@
         <v>-7.2169999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>-3</v>
       </c>
@@ -5598,7 +5643,7 @@
         <v>-5.625</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>-2</v>
       </c>
@@ -5606,7 +5651,7 @@
         <v>-3.9550000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>-1</v>
       </c>
@@ -5614,7 +5659,7 @@
         <v>-2.2850000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5622,7 +5667,7 @@
         <v>-0.59079999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5630,7 +5675,7 @@
         <v>1.0640000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -5638,7 +5683,7 @@
         <v>2.7389999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -5646,7 +5691,7 @@
         <v>4.3849999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -5654,7 +5699,7 @@
         <v>6.0449999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -5665,7 +5710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>-10</v>
       </c>
@@ -5677,7 +5722,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>-9</v>
       </c>
@@ -5689,7 +5734,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>-8</v>
       </c>
@@ -5701,7 +5746,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>-7</v>
       </c>
@@ -5713,7 +5758,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>-6</v>
       </c>
@@ -5725,7 +5770,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>-5</v>
       </c>
@@ -5737,7 +5782,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>-4</v>
       </c>
@@ -5749,7 +5794,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>-3</v>
       </c>
@@ -5761,7 +5806,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>-2</v>
       </c>
@@ -5773,7 +5818,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>-1</v>
       </c>
@@ -5785,7 +5830,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>-0.75</v>
       </c>
@@ -5797,7 +5842,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>-0.5</v>
       </c>
@@ -5809,7 +5854,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>-0.25</v>
       </c>
@@ -5821,7 +5866,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -5833,7 +5878,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0.25</v>
       </c>
@@ -5845,7 +5890,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0.5</v>
       </c>
@@ -5857,7 +5902,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0.75</v>
       </c>
@@ -5869,7 +5914,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -5881,7 +5926,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -5893,7 +5938,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -5905,7 +5950,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -5917,7 +5962,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>5</v>
       </c>
@@ -5929,7 +5974,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>6</v>
       </c>
@@ -5941,7 +5986,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7</v>
       </c>
@@ -5953,7 +5998,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -5965,7 +6010,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>9</v>
       </c>
@@ -5977,7 +6022,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10</v>
       </c>
@@ -5989,12 +6034,12 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -6002,12 +6047,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -6015,7 +6060,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -6023,7 +6068,7 @@
         <v>4.3049999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -6035,4 +6080,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E0A3CF-FDA7-4717-85B0-E8F3EB4F0CB2}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1">
+        <f>-1.703-(-2)</f>
+        <v>0.29699999999999993</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <f>D1/2</f>
+        <v>0.14849999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f>2-1.882</f>
+        <v>0.1180000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>